<commit_message>
improvements: filtering for hiding roles (first implementation); samples files have been updated
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.f.xlsx
+++ b/example/Estimation Tool.mm.f.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$76</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$76</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
   <si>
     <t xml:space="preserve">Task / Subtask</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Filter</t>
   </si>
   <si>
     <t xml:space="preserve">Comment</t>
@@ -398,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,10 +426,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -436,10 +435,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -467,10 +462,6 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,19 +470,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -620,63 +603,63 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H1" s="4"/>
       <c r="I1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="6" t="n">
-        <v>0</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="B2" s="5"/>
       <c r="C2" s="5"/>
-      <c r="D2" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="8" t="n">
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="7" t="n">
         <f aca="false">E3+E12+E17+E19</f>
         <v>8</v>
       </c>
-      <c r="F2" s="8" t="n">
+      <c r="F2" s="7" t="n">
         <f aca="false">F3+F12+F17+F19</f>
         <v>13</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="7" t="n">
         <f aca="false">G3+G12+G17+G19</f>
         <v>27</v>
       </c>
@@ -690,30 +673,28 @@
       <c r="P2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12" t="n">
+      <c r="A3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10" t="n">
         <f aca="false">E4+E6+E8+E10</f>
         <v>3</v>
       </c>
-      <c r="F3" s="12" t="n">
+      <c r="F3" s="10" t="n">
         <f aca="false">F4+F6+F8+F10</f>
         <v>6</v>
       </c>
-      <c r="G3" s="12" t="n">
+      <c r="G3" s="10" t="n">
         <f aca="false">G4+G6+G8+G10</f>
         <v>13</v>
       </c>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
@@ -721,32 +702,32 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="13" t="n">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="n">
         <f aca="false">E5</f>
         <v>1</v>
       </c>
-      <c r="F4" s="13" t="n">
+      <c r="F4" s="11" t="n">
         <f aca="false">F5</f>
         <v>1</v>
       </c>
-      <c r="G4" s="13" t="n">
+      <c r="G4" s="11" t="n">
         <f aca="false">G5</f>
         <v>2</v>
       </c>
-      <c r="I4" s="13" t="n">
+      <c r="I4" s="11" t="n">
         <f aca="false">(E4+4*F4+G4)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J4" s="13" t="n">
+      <c r="J4" s="11" t="n">
         <f aca="false">(G4-E4)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K4" s="13" t="n">
+      <c r="K4" s="11" t="n">
         <f aca="false">J4*J4</f>
         <v>0.0277777777777778</v>
       </c>
@@ -756,21 +737,21 @@
       <c r="P4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="15" t="n">
+      <c r="A5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H5" s="0"/>
@@ -786,32 +767,32 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" s="13" t="n">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="11" t="n">
         <f aca="false">E7</f>
         <v>1</v>
       </c>
-      <c r="F6" s="13" t="n">
+      <c r="F6" s="11" t="n">
         <f aca="false">F7</f>
         <v>2</v>
       </c>
-      <c r="G6" s="13" t="n">
+      <c r="G6" s="11" t="n">
         <f aca="false">G7</f>
         <v>4</v>
       </c>
-      <c r="I6" s="13" t="n">
+      <c r="I6" s="11" t="n">
         <f aca="false">(E6+4*F6+G6)/6</f>
         <v>2.16666666666667</v>
       </c>
-      <c r="J6" s="13" t="n">
+      <c r="J6" s="11" t="n">
         <f aca="false">(G6-E6)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K6" s="13" t="n">
+      <c r="K6" s="11" t="n">
         <f aca="false">J6*J6</f>
         <v>0.25</v>
       </c>
@@ -821,21 +802,21 @@
       <c r="P6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="15" t="n">
+      <c r="A7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="13" t="n">
         <v>4</v>
       </c>
       <c r="H7" s="0"/>
@@ -851,32 +832,32 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13" t="n">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="11" t="n">
         <f aca="false">E9</f>
         <v>1</v>
       </c>
-      <c r="F8" s="13" t="n">
+      <c r="F8" s="11" t="n">
         <f aca="false">F9</f>
         <v>2</v>
       </c>
-      <c r="G8" s="13" t="n">
+      <c r="G8" s="11" t="n">
         <f aca="false">G9</f>
         <v>4</v>
       </c>
-      <c r="I8" s="13" t="n">
+      <c r="I8" s="11" t="n">
         <f aca="false">(E8+4*F8+G8)/6</f>
         <v>2.16666666666667</v>
       </c>
-      <c r="J8" s="13" t="n">
+      <c r="J8" s="11" t="n">
         <f aca="false">(G8-E8)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K8" s="13" t="n">
+      <c r="K8" s="11" t="n">
         <f aca="false">J8*J8</f>
         <v>0.25</v>
       </c>
@@ -886,21 +867,21 @@
       <c r="P8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G9" s="15" t="n">
+      <c r="A9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="13" t="n">
         <v>4</v>
       </c>
       <c r="H9" s="0"/>
@@ -916,32 +897,32 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" s="13" t="n">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E10" s="11" t="n">
         <f aca="false">E11</f>
         <v>0</v>
       </c>
-      <c r="F10" s="13" t="n">
+      <c r="F10" s="11" t="n">
         <f aca="false">F11</f>
         <v>1</v>
       </c>
-      <c r="G10" s="13" t="n">
+      <c r="G10" s="11" t="n">
         <f aca="false">G11</f>
         <v>3</v>
       </c>
-      <c r="I10" s="13" t="n">
+      <c r="I10" s="11" t="n">
         <f aca="false">(E10+4*F10+G10)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J10" s="13" t="n">
+      <c r="J10" s="11" t="n">
         <f aca="false">(G10-E10)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K10" s="13" t="n">
+      <c r="K10" s="11" t="n">
         <f aca="false">J10*J10</f>
         <v>0.25</v>
       </c>
@@ -951,21 +932,21 @@
       <c r="P10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="15" t="n">
+      <c r="A11" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="13" t="n">
         <v>3</v>
       </c>
       <c r="H11" s="0"/>
@@ -980,30 +961,28 @@
       <c r="P11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="12" t="n">
+      <c r="A12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="n">
         <f aca="false">E13+E15</f>
         <v>3</v>
       </c>
-      <c r="F12" s="12" t="n">
+      <c r="F12" s="10" t="n">
         <f aca="false">F13+F15</f>
         <v>4</v>
       </c>
-      <c r="G12" s="12" t="n">
+      <c r="G12" s="10" t="n">
         <f aca="false">G13+G15</f>
         <v>7</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
@@ -1011,32 +990,32 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" s="13" t="n">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E13" s="11" t="n">
         <f aca="false">E14</f>
         <v>1</v>
       </c>
-      <c r="F13" s="13" t="n">
+      <c r="F13" s="11" t="n">
         <f aca="false">F14</f>
         <v>1</v>
       </c>
-      <c r="G13" s="13" t="n">
+      <c r="G13" s="11" t="n">
         <f aca="false">G14</f>
         <v>2</v>
       </c>
-      <c r="I13" s="13" t="n">
+      <c r="I13" s="11" t="n">
         <f aca="false">(E13+4*F13+G13)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J13" s="13" t="n">
+      <c r="J13" s="11" t="n">
         <f aca="false">(G13-E13)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K13" s="13" t="n">
+      <c r="K13" s="11" t="n">
         <f aca="false">J13*J13</f>
         <v>0.0277777777777778</v>
       </c>
@@ -1046,21 +1025,21 @@
       <c r="P13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F14" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="15" t="n">
+      <c r="A14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H14" s="0"/>
@@ -1076,32 +1055,32 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" s="13" t="n">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E15" s="11" t="n">
         <f aca="false">E16</f>
         <v>2</v>
       </c>
-      <c r="F15" s="13" t="n">
+      <c r="F15" s="11" t="n">
         <f aca="false">F16</f>
         <v>3</v>
       </c>
-      <c r="G15" s="13" t="n">
+      <c r="G15" s="11" t="n">
         <f aca="false">G16</f>
         <v>5</v>
       </c>
-      <c r="I15" s="13" t="n">
+      <c r="I15" s="11" t="n">
         <f aca="false">(E15+4*F15+G15)/6</f>
         <v>3.16666666666667</v>
       </c>
-      <c r="J15" s="13" t="n">
+      <c r="J15" s="11" t="n">
         <f aca="false">(G15-E15)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K15" s="13" t="n">
+      <c r="K15" s="11" t="n">
         <f aca="false">J15*J15</f>
         <v>0.25</v>
       </c>
@@ -1111,21 +1090,21 @@
       <c r="P15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F16" s="15" t="n">
+      <c r="A16" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="15" t="n">
+      <c r="G16" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H16" s="0"/>
@@ -1141,32 +1120,32 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" s="13" t="n">
+        <v>25</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E17" s="11" t="n">
         <f aca="false">E18</f>
         <v>1</v>
       </c>
-      <c r="F17" s="13" t="n">
+      <c r="F17" s="11" t="n">
         <f aca="false">F18</f>
         <v>2</v>
       </c>
-      <c r="G17" s="13" t="n">
+      <c r="G17" s="11" t="n">
         <f aca="false">G18</f>
         <v>5</v>
       </c>
-      <c r="I17" s="13" t="n">
+      <c r="I17" s="11" t="n">
         <f aca="false">(E17+4*F17+G17)/6</f>
         <v>2.33333333333333</v>
       </c>
-      <c r="J17" s="13" t="n">
+      <c r="J17" s="11" t="n">
         <f aca="false">(G17-E17)/6</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="K17" s="13" t="n">
+      <c r="K17" s="11" t="n">
         <f aca="false">J17*J17</f>
         <v>0.444444444444444</v>
       </c>
@@ -1176,21 +1155,21 @@
       <c r="P17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F18" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="15" t="n">
+      <c r="A18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H18" s="0"/>
@@ -1206,32 +1185,32 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" s="13" t="n">
+        <v>27</v>
+      </c>
+      <c r="B19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11" t="n">
         <f aca="false">E20</f>
         <v>1</v>
       </c>
-      <c r="F19" s="13" t="n">
+      <c r="F19" s="11" t="n">
         <f aca="false">F20</f>
         <v>1</v>
       </c>
-      <c r="G19" s="13" t="n">
+      <c r="G19" s="11" t="n">
         <f aca="false">G20</f>
         <v>2</v>
       </c>
-      <c r="I19" s="13" t="n">
+      <c r="I19" s="11" t="n">
         <f aca="false">(E19+4*F19+G19)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J19" s="13" t="n">
+      <c r="J19" s="11" t="n">
         <f aca="false">(G19-E19)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K19" s="13" t="n">
+      <c r="K19" s="11" t="n">
         <f aca="false">J19*J19</f>
         <v>0.0277777777777778</v>
       </c>
@@ -1241,21 +1220,21 @@
       <c r="P19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F20" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G20" s="15" t="n">
+      <c r="A20" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H20" s="0"/>
@@ -1271,24 +1250,22 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="6" t="n">
-        <v>0</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B21" s="5"/>
       <c r="C21" s="5"/>
-      <c r="D21" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="8" t="n">
+      <c r="D21" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="7" t="n">
         <f aca="false">E22+E29+E32</f>
         <v>7</v>
       </c>
-      <c r="F21" s="8" t="n">
+      <c r="F21" s="7" t="n">
         <f aca="false">F22+F29+F32</f>
         <v>16</v>
       </c>
-      <c r="G21" s="8" t="n">
+      <c r="G21" s="7" t="n">
         <f aca="false">G22+G29+G32</f>
         <v>27</v>
       </c>
@@ -1302,32 +1279,30 @@
       <c r="P21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="11" t="s">
+      <c r="A22" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="12" t="n">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="10" t="n">
         <f aca="false">E23+E25+E27</f>
         <v>6</v>
       </c>
-      <c r="F22" s="12" t="n">
+      <c r="F22" s="10" t="n">
         <f aca="false">F23+F25+F27</f>
         <v>9</v>
       </c>
-      <c r="G22" s="12" t="n">
+      <c r="G22" s="10" t="n">
         <f aca="false">G23+G25+G27</f>
         <v>15</v>
       </c>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
       <c r="O22" s="0"/>
@@ -1335,32 +1310,32 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E23" s="13" t="n">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E23" s="11" t="n">
         <f aca="false">E24</f>
         <v>3</v>
       </c>
-      <c r="F23" s="13" t="n">
+      <c r="F23" s="11" t="n">
         <f aca="false">F24</f>
         <v>5</v>
       </c>
-      <c r="G23" s="13" t="n">
+      <c r="G23" s="11" t="n">
         <f aca="false">G24</f>
         <v>10</v>
       </c>
-      <c r="I23" s="13" t="n">
+      <c r="I23" s="11" t="n">
         <f aca="false">(E23+4*F23+G23)/6</f>
         <v>5.5</v>
       </c>
-      <c r="J23" s="13" t="n">
+      <c r="J23" s="11" t="n">
         <f aca="false">(G23-E23)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="K23" s="13" t="n">
+      <c r="K23" s="11" t="n">
         <f aca="false">J23*J23</f>
         <v>1.36111111111111</v>
       </c>
@@ -1370,21 +1345,21 @@
       <c r="P23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B24" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="15" t="n">
+      <c r="A24" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="F24" s="15" t="n">
+      <c r="F24" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="G24" s="15" t="n">
+      <c r="G24" s="13" t="n">
         <v>10</v>
       </c>
       <c r="H24" s="0"/>
@@ -1400,32 +1375,32 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E25" s="13" t="n">
+        <v>33</v>
+      </c>
+      <c r="B25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" s="11" t="n">
         <f aca="false">E26</f>
         <v>2</v>
       </c>
-      <c r="F25" s="13" t="n">
+      <c r="F25" s="11" t="n">
         <f aca="false">F26</f>
         <v>2</v>
       </c>
-      <c r="G25" s="13" t="n">
+      <c r="G25" s="11" t="n">
         <f aca="false">G26</f>
         <v>3</v>
       </c>
-      <c r="I25" s="13" t="n">
+      <c r="I25" s="11" t="n">
         <f aca="false">(E25+4*F25+G25)/6</f>
         <v>2.16666666666667</v>
       </c>
-      <c r="J25" s="13" t="n">
+      <c r="J25" s="11" t="n">
         <f aca="false">(G25-E25)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K25" s="13" t="n">
+      <c r="K25" s="11" t="n">
         <f aca="false">J25*J25</f>
         <v>0.0277777777777778</v>
       </c>
@@ -1435,21 +1410,21 @@
       <c r="P25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B26" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F26" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G26" s="15" t="n">
+      <c r="A26" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F26" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G26" s="13" t="n">
         <v>3</v>
       </c>
       <c r="H26" s="0"/>
@@ -1465,32 +1440,32 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E27" s="13" t="n">
+        <v>34</v>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E27" s="11" t="n">
         <f aca="false">E28</f>
         <v>1</v>
       </c>
-      <c r="F27" s="13" t="n">
+      <c r="F27" s="11" t="n">
         <f aca="false">F28</f>
         <v>2</v>
       </c>
-      <c r="G27" s="13" t="n">
+      <c r="G27" s="11" t="n">
         <f aca="false">G28</f>
         <v>2</v>
       </c>
-      <c r="I27" s="13" t="n">
+      <c r="I27" s="11" t="n">
         <f aca="false">(E27+4*F27+G27)/6</f>
         <v>1.83333333333333</v>
       </c>
-      <c r="J27" s="13" t="n">
+      <c r="J27" s="11" t="n">
         <f aca="false">(G27-E27)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K27" s="13" t="n">
+      <c r="K27" s="11" t="n">
         <f aca="false">J27*J27</f>
         <v>0.0277777777777778</v>
       </c>
@@ -1500,21 +1475,21 @@
       <c r="P27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B28" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F28" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G28" s="15" t="n">
+      <c r="A28" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G28" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H28" s="0"/>
@@ -1530,32 +1505,32 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E29" s="13" t="n">
+        <v>35</v>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E29" s="11" t="n">
         <f aca="false">E30+E31</f>
         <v>1</v>
       </c>
-      <c r="F29" s="13" t="n">
+      <c r="F29" s="11" t="n">
         <f aca="false">F30+F31</f>
         <v>3</v>
       </c>
-      <c r="G29" s="13" t="n">
+      <c r="G29" s="11" t="n">
         <f aca="false">G30+G31</f>
         <v>5</v>
       </c>
-      <c r="I29" s="13" t="n">
+      <c r="I29" s="11" t="n">
         <f aca="false">(E29+4*F29+G29)/6</f>
         <v>3</v>
       </c>
-      <c r="J29" s="13" t="n">
+      <c r="J29" s="11" t="n">
         <f aca="false">(G29-E29)/6</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="K29" s="13" t="n">
+      <c r="K29" s="11" t="n">
         <f aca="false">J29*J29</f>
         <v>0.444444444444444</v>
       </c>
@@ -1565,21 +1540,21 @@
       <c r="P29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F30" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G30" s="15" t="n">
+      <c r="A30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" s="12"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G30" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H30" s="0"/>
@@ -1594,21 +1569,21 @@
       <c r="P30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B31" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G31" s="15" t="n">
+      <c r="A31" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G31" s="13" t="n">
         <v>3</v>
       </c>
       <c r="H31" s="0"/>
@@ -1624,32 +1599,32 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E32" s="13" t="n">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" s="11" t="n">
         <f aca="false">E33+E34</f>
         <v>0</v>
       </c>
-      <c r="F32" s="13" t="n">
+      <c r="F32" s="11" t="n">
         <f aca="false">F33+F34</f>
         <v>4</v>
       </c>
-      <c r="G32" s="13" t="n">
+      <c r="G32" s="11" t="n">
         <f aca="false">G33+G34</f>
         <v>7</v>
       </c>
-      <c r="I32" s="13" t="n">
+      <c r="I32" s="11" t="n">
         <f aca="false">(E32+4*F32+G32)/6</f>
         <v>3.83333333333333</v>
       </c>
-      <c r="J32" s="13" t="n">
+      <c r="J32" s="11" t="n">
         <f aca="false">(G32-E32)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="K32" s="13" t="n">
+      <c r="K32" s="11" t="n">
         <f aca="false">J32*J32</f>
         <v>1.36111111111111</v>
       </c>
@@ -1659,21 +1634,21 @@
       <c r="P32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B33" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="15" t="n">
+      <c r="A33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H33" s="0"/>
@@ -1688,21 +1663,21 @@
       <c r="P33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" s="15" t="n">
+      <c r="A34" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G34" s="15" t="n">
+      <c r="G34" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H34" s="0"/>
@@ -1718,24 +1693,22 @@
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="6" t="n">
-        <v>0</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E35" s="8" t="n">
+      <c r="D35" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" s="7" t="n">
         <f aca="false">E36+E41+E43+E45+E47</f>
         <v>8</v>
       </c>
-      <c r="F35" s="8" t="n">
+      <c r="F35" s="7" t="n">
         <f aca="false">F36+F41+F43+F45+F47</f>
         <v>12</v>
       </c>
-      <c r="G35" s="8" t="n">
+      <c r="G35" s="7" t="n">
         <f aca="false">G36+G41+G43+G45+G47</f>
         <v>21</v>
       </c>
@@ -1749,30 +1722,28 @@
       <c r="P35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C36" s="9"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="12" t="n">
+      <c r="A36" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10" t="n">
         <f aca="false">E37+E39</f>
         <v>3</v>
       </c>
-      <c r="F36" s="12" t="n">
+      <c r="F36" s="10" t="n">
         <f aca="false">F37+F39</f>
         <v>5</v>
       </c>
-      <c r="G36" s="12" t="n">
+      <c r="G36" s="10" t="n">
         <f aca="false">G37+G39</f>
         <v>10</v>
       </c>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9"/>
-      <c r="K36" s="9"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
       <c r="O36" s="0"/>
@@ -1780,32 +1751,32 @@
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E37" s="13" t="n">
+        <v>41</v>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E37" s="11" t="n">
         <f aca="false">E38</f>
         <v>1</v>
       </c>
-      <c r="F37" s="13" t="n">
+      <c r="F37" s="11" t="n">
         <f aca="false">F38</f>
         <v>2</v>
       </c>
-      <c r="G37" s="13" t="n">
+      <c r="G37" s="11" t="n">
         <f aca="false">G38</f>
         <v>5</v>
       </c>
-      <c r="I37" s="13" t="n">
+      <c r="I37" s="11" t="n">
         <f aca="false">(E37+4*F37+G37)/6</f>
         <v>2.33333333333333</v>
       </c>
-      <c r="J37" s="13" t="n">
+      <c r="J37" s="11" t="n">
         <f aca="false">(G37-E37)/6</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="K37" s="13" t="n">
+      <c r="K37" s="11" t="n">
         <f aca="false">J37*J37</f>
         <v>0.444444444444444</v>
       </c>
@@ -1815,21 +1786,21 @@
       <c r="P37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F38" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="G38" s="15" t="n">
+      <c r="A38" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="G38" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H38" s="0"/>
@@ -1845,32 +1816,32 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E39" s="13" t="n">
+        <v>42</v>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E39" s="11" t="n">
         <f aca="false">E40</f>
         <v>2</v>
       </c>
-      <c r="F39" s="13" t="n">
+      <c r="F39" s="11" t="n">
         <f aca="false">F40</f>
         <v>3</v>
       </c>
-      <c r="G39" s="13" t="n">
+      <c r="G39" s="11" t="n">
         <f aca="false">G40</f>
         <v>5</v>
       </c>
-      <c r="I39" s="13" t="n">
+      <c r="I39" s="11" t="n">
         <f aca="false">(E39+4*F39+G39)/6</f>
         <v>3.16666666666667</v>
       </c>
-      <c r="J39" s="13" t="n">
+      <c r="J39" s="11" t="n">
         <f aca="false">(G39-E39)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K39" s="13" t="n">
+      <c r="K39" s="11" t="n">
         <f aca="false">J39*J39</f>
         <v>0.25</v>
       </c>
@@ -1880,21 +1851,21 @@
       <c r="P39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F40" s="15" t="n">
+      <c r="A40" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B40" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F40" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G40" s="15" t="n">
+      <c r="G40" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H40" s="0"/>
@@ -1910,32 +1881,32 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E41" s="13" t="n">
+        <v>43</v>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="11" t="n">
         <f aca="false">E42</f>
         <v>1</v>
       </c>
-      <c r="F41" s="13" t="n">
+      <c r="F41" s="11" t="n">
         <f aca="false">F42</f>
         <v>1</v>
       </c>
-      <c r="G41" s="13" t="n">
+      <c r="G41" s="11" t="n">
         <f aca="false">G42</f>
         <v>2</v>
       </c>
-      <c r="I41" s="13" t="n">
+      <c r="I41" s="11" t="n">
         <f aca="false">(E41+4*F41+G41)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J41" s="13" t="n">
+      <c r="J41" s="11" t="n">
         <f aca="false">(G41-E41)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K41" s="13" t="n">
+      <c r="K41" s="11" t="n">
         <f aca="false">J41*J41</f>
         <v>0.0277777777777778</v>
       </c>
@@ -1945,21 +1916,21 @@
       <c r="P41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F42" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G42" s="15" t="n">
+      <c r="A42" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F42" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G42" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H42" s="0"/>
@@ -1975,32 +1946,32 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E43" s="13" t="n">
+        <v>45</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="11" t="n">
         <f aca="false">E44</f>
         <v>2</v>
       </c>
-      <c r="F43" s="13" t="n">
+      <c r="F43" s="11" t="n">
         <f aca="false">F44</f>
         <v>4</v>
       </c>
-      <c r="G43" s="13" t="n">
+      <c r="G43" s="11" t="n">
         <f aca="false">G44</f>
         <v>5</v>
       </c>
-      <c r="I43" s="13" t="n">
+      <c r="I43" s="11" t="n">
         <f aca="false">(E43+4*F43+G43)/6</f>
         <v>3.83333333333333</v>
       </c>
-      <c r="J43" s="13" t="n">
+      <c r="J43" s="11" t="n">
         <f aca="false">(G43-E43)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K43" s="13" t="n">
+      <c r="K43" s="11" t="n">
         <f aca="false">J43*J43</f>
         <v>0.25</v>
       </c>
@@ -2009,21 +1980,21 @@
       <c r="P43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B44" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F44" s="15" t="n">
+      <c r="A44" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C44" s="12"/>
+      <c r="D44" s="12"/>
+      <c r="E44" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F44" s="13" t="n">
         <v>4</v>
       </c>
-      <c r="G44" s="15" t="n">
+      <c r="G44" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H44" s="0"/>
@@ -2038,32 +2009,32 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B45" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E45" s="13" t="n">
+        <v>46</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E45" s="11" t="n">
         <f aca="false">E46</f>
         <v>1</v>
       </c>
-      <c r="F45" s="13" t="n">
+      <c r="F45" s="11" t="n">
         <f aca="false">F46</f>
         <v>1</v>
       </c>
-      <c r="G45" s="13" t="n">
+      <c r="G45" s="11" t="n">
         <f aca="false">G46</f>
         <v>2</v>
       </c>
-      <c r="I45" s="13" t="n">
+      <c r="I45" s="11" t="n">
         <f aca="false">(E45+4*F45+G45)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J45" s="13" t="n">
+      <c r="J45" s="11" t="n">
         <f aca="false">(G45-E45)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K45" s="13" t="n">
+      <c r="K45" s="11" t="n">
         <f aca="false">J45*J45</f>
         <v>0.0277777777777778</v>
       </c>
@@ -2072,21 +2043,21 @@
       <c r="P45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B46" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F46" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G46" s="15" t="n">
+      <c r="A46" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G46" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H46" s="0"/>
@@ -2101,35 +2072,35 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="B47" s="1" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E47" s="13" t="n">
+        <v>48</v>
+      </c>
+      <c r="E47" s="11" t="n">
         <f aca="false">E48</f>
         <v>1</v>
       </c>
-      <c r="F47" s="13" t="n">
+      <c r="F47" s="11" t="n">
         <f aca="false">F48</f>
         <v>1</v>
       </c>
-      <c r="G47" s="13" t="n">
+      <c r="G47" s="11" t="n">
         <f aca="false">G48</f>
         <v>2</v>
       </c>
-      <c r="I47" s="13" t="n">
+      <c r="I47" s="11" t="n">
         <f aca="false">(E47+4*F47+G47)/6</f>
         <v>1.16666666666667</v>
       </c>
-      <c r="J47" s="13" t="n">
+      <c r="J47" s="11" t="n">
         <f aca="false">(G47-E47)/6</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="K47" s="13" t="n">
+      <c r="K47" s="11" t="n">
         <f aca="false">J47*J47</f>
         <v>0.0277777777777778</v>
       </c>
@@ -2138,21 +2109,21 @@
       <c r="P47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B48" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="15" t="n">
+      <c r="A48" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C48" s="12"/>
+      <c r="D48" s="12"/>
+      <c r="E48" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="13" t="n">
         <v>2</v>
       </c>
       <c r="H48" s="0"/>
@@ -2167,24 +2138,22 @@
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B49" s="6" t="n">
-        <v>0</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E49" s="8" t="n">
+      <c r="D49" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" s="7" t="n">
         <f aca="false">E50+E52+E54</f>
         <v>4</v>
       </c>
-      <c r="F49" s="8" t="n">
+      <c r="F49" s="7" t="n">
         <f aca="false">F50+F52+F54</f>
         <v>13</v>
       </c>
-      <c r="G49" s="8" t="n">
+      <c r="G49" s="7" t="n">
         <f aca="false">G50+G52+G54</f>
         <v>28</v>
       </c>
@@ -2198,32 +2167,32 @@
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E50" s="13" t="n">
+        <v>51</v>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E50" s="11" t="n">
         <f aca="false">E51</f>
         <v>2</v>
       </c>
-      <c r="F50" s="13" t="n">
+      <c r="F50" s="11" t="n">
         <f aca="false">F51</f>
         <v>3</v>
       </c>
-      <c r="G50" s="13" t="n">
+      <c r="G50" s="11" t="n">
         <f aca="false">G51</f>
         <v>5</v>
       </c>
-      <c r="I50" s="13" t="n">
+      <c r="I50" s="11" t="n">
         <f aca="false">(E50+4*F50+G50)/6</f>
         <v>3.16666666666667</v>
       </c>
-      <c r="J50" s="13" t="n">
+      <c r="J50" s="11" t="n">
         <f aca="false">(G50-E50)/6</f>
         <v>0.5</v>
       </c>
-      <c r="K50" s="13" t="n">
+      <c r="K50" s="11" t="n">
         <f aca="false">J50*J50</f>
         <v>0.25</v>
       </c>
@@ -2232,21 +2201,21 @@
       <c r="P50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B51" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F51" s="15" t="n">
+      <c r="A51" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C51" s="12"/>
+      <c r="D51" s="12"/>
+      <c r="E51" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F51" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="G51" s="15" t="n">
+      <c r="G51" s="13" t="n">
         <v>5</v>
       </c>
       <c r="H51" s="0"/>
@@ -2261,32 +2230,32 @@
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B52" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" s="13" t="n">
+        <v>52</v>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" s="11" t="n">
         <f aca="false">E53</f>
         <v>2</v>
       </c>
-      <c r="F52" s="13" t="n">
+      <c r="F52" s="11" t="n">
         <f aca="false">F53</f>
         <v>5</v>
       </c>
-      <c r="G52" s="13" t="n">
+      <c r="G52" s="11" t="n">
         <f aca="false">G53</f>
         <v>8</v>
       </c>
-      <c r="I52" s="13" t="n">
+      <c r="I52" s="11" t="n">
         <f aca="false">(E52+4*F52+G52)/6</f>
         <v>5</v>
       </c>
-      <c r="J52" s="13" t="n">
+      <c r="J52" s="11" t="n">
         <f aca="false">(G52-E52)/6</f>
         <v>1</v>
       </c>
-      <c r="K52" s="13" t="n">
+      <c r="K52" s="11" t="n">
         <f aca="false">J52*J52</f>
         <v>1</v>
       </c>
@@ -2295,21 +2264,21 @@
       <c r="P52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B53" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="15" t="n">
-        <v>2</v>
-      </c>
-      <c r="F53" s="15" t="n">
+      <c r="A53" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
+      <c r="E53" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="F53" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="G53" s="15" t="n">
+      <c r="G53" s="13" t="n">
         <v>8</v>
       </c>
       <c r="H53" s="0"/>
@@ -2324,32 +2293,32 @@
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B54" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E54" s="13" t="n">
+        <v>37</v>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E54" s="11" t="n">
         <f aca="false">E55</f>
         <v>0</v>
       </c>
-      <c r="F54" s="13" t="n">
+      <c r="F54" s="11" t="n">
         <f aca="false">F55</f>
         <v>5</v>
       </c>
-      <c r="G54" s="13" t="n">
+      <c r="G54" s="11" t="n">
         <f aca="false">G55</f>
         <v>15</v>
       </c>
-      <c r="I54" s="13" t="n">
+      <c r="I54" s="11" t="n">
         <f aca="false">(E54+4*F54+G54)/6</f>
         <v>5.83333333333333</v>
       </c>
-      <c r="J54" s="13" t="n">
+      <c r="J54" s="11" t="n">
         <f aca="false">(G54-E54)/6</f>
         <v>2.5</v>
       </c>
-      <c r="K54" s="13" t="n">
+      <c r="K54" s="11" t="n">
         <f aca="false">J54*J54</f>
         <v>6.25</v>
       </c>
@@ -2357,21 +2326,21 @@
       <c r="P54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" s="15" t="n">
+      <c r="A55" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B55" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F55" s="13" t="n">
         <v>5</v>
       </c>
-      <c r="G55" s="15" t="n">
+      <c r="G55" s="13" t="n">
         <v>15</v>
       </c>
       <c r="H55" s="0"/>
@@ -2385,24 +2354,22 @@
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B56" s="6" t="n">
-        <v>0</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="B56" s="5"/>
       <c r="C56" s="5"/>
-      <c r="D56" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E56" s="8" t="n">
+      <c r="D56" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E56" s="7" t="n">
         <f aca="false">E57</f>
         <v>0</v>
       </c>
-      <c r="F56" s="8" t="n">
+      <c r="F56" s="7" t="n">
         <f aca="false">F57</f>
         <v>0</v>
       </c>
-      <c r="G56" s="8" t="n">
+      <c r="G56" s="7" t="n">
         <f aca="false">G57</f>
         <v>0</v>
       </c>
@@ -2413,129 +2380,118 @@
       <c r="P56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="C57" s="9"/>
-      <c r="D57" s="11"/>
-      <c r="E57" s="12" t="n">
+      <c r="A57" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10" t="n">
         <f aca="false">E58+E73</f>
         <v>0</v>
       </c>
-      <c r="F57" s="12" t="n">
+      <c r="F57" s="10" t="n">
         <f aca="false">F58+F73</f>
         <v>0</v>
       </c>
-      <c r="G57" s="12" t="n">
+      <c r="G57" s="10" t="n">
         <f aca="false">G58+G73</f>
         <v>0</v>
       </c>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
-      <c r="J57" s="9"/>
-      <c r="K57" s="9"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
       <c r="P57" s="0"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B58" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
-      <c r="E58" s="18" t="n">
+      <c r="A58" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="15" t="n">
         <f aca="false">E59+E68</f>
         <v>0</v>
       </c>
-      <c r="F58" s="18" t="n">
+      <c r="F58" s="15" t="n">
         <f aca="false">F59+F68</f>
         <v>0</v>
       </c>
-      <c r="G58" s="18" t="n">
+      <c r="G58" s="15" t="n">
         <f aca="false">G59+G68</f>
         <v>0</v>
       </c>
-      <c r="H58" s="16"/>
-      <c r="I58" s="16"/>
-      <c r="J58" s="16"/>
-      <c r="K58" s="16"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+      <c r="K58" s="14"/>
       <c r="P58" s="0"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B59" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" s="19"/>
-      <c r="D59" s="19"/>
-      <c r="E59" s="21" t="n">
+      <c r="A59" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="16"/>
+      <c r="C59" s="16"/>
+      <c r="D59" s="16"/>
+      <c r="E59" s="17" t="n">
         <f aca="false">E60</f>
         <v>0</v>
       </c>
-      <c r="F59" s="21" t="n">
+      <c r="F59" s="17" t="n">
         <f aca="false">F60</f>
         <v>0</v>
       </c>
-      <c r="G59" s="21" t="n">
+      <c r="G59" s="17" t="n">
         <f aca="false">G60</f>
         <v>0</v>
       </c>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="16"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
       <c r="P59" s="0"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B60" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C60" s="22"/>
-      <c r="D60" s="22"/>
-      <c r="E60" s="24" t="n">
+      <c r="A60" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="18"/>
+      <c r="C60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="19" t="n">
         <f aca="false">E61</f>
         <v>0</v>
       </c>
-      <c r="F60" s="24" t="n">
+      <c r="F60" s="19" t="n">
         <f aca="false">F61</f>
         <v>0</v>
       </c>
-      <c r="G60" s="24" t="n">
+      <c r="G60" s="19" t="n">
         <f aca="false">G61</f>
         <v>0</v>
       </c>
-      <c r="H60" s="22"/>
-      <c r="I60" s="22"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="22"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
       <c r="P60" s="0"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B61" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E61" s="15" t="n">
+        <v>59</v>
+      </c>
+      <c r="E61" s="13" t="n">
         <f aca="false">E62+E66</f>
         <v>0</v>
       </c>
-      <c r="F61" s="15" t="n">
+      <c r="F61" s="13" t="n">
         <f aca="false">F62+F66</f>
         <v>0</v>
       </c>
-      <c r="G61" s="15" t="n">
+      <c r="G61" s="13" t="n">
         <f aca="false">G62+G66</f>
         <v>0</v>
       </c>
@@ -2546,20 +2502,17 @@
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B62" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E62" s="15" t="n">
+        <v>60</v>
+      </c>
+      <c r="E62" s="13" t="n">
         <f aca="false">E63</f>
         <v>0</v>
       </c>
-      <c r="F62" s="15" t="n">
+      <c r="F62" s="13" t="n">
         <f aca="false">F63</f>
         <v>0</v>
       </c>
-      <c r="G62" s="15" t="n">
+      <c r="G62" s="13" t="n">
         <f aca="false">G63</f>
         <v>0</v>
       </c>
@@ -2570,20 +2523,17 @@
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B63" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E63" s="15" t="n">
+        <v>61</v>
+      </c>
+      <c r="E63" s="13" t="n">
         <f aca="false">E64</f>
         <v>0</v>
       </c>
-      <c r="F63" s="15" t="n">
+      <c r="F63" s="13" t="n">
         <f aca="false">F64</f>
         <v>0</v>
       </c>
-      <c r="G63" s="15" t="n">
+      <c r="G63" s="13" t="n">
         <f aca="false">G64</f>
         <v>0</v>
       </c>
@@ -2594,53 +2544,53 @@
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B64" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="13" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E64" s="11" t="n">
         <f aca="false">E65</f>
         <v>0</v>
       </c>
-      <c r="F64" s="13" t="n">
+      <c r="F64" s="11" t="n">
         <f aca="false">F65</f>
         <v>0</v>
       </c>
-      <c r="G64" s="13" t="n">
+      <c r="G64" s="11" t="n">
         <f aca="false">G65</f>
         <v>0</v>
       </c>
-      <c r="I64" s="13" t="n">
+      <c r="I64" s="11" t="n">
         <f aca="false">(E64+4*F64+G64)/6</f>
         <v>0</v>
       </c>
-      <c r="J64" s="13" t="n">
+      <c r="J64" s="11" t="n">
         <f aca="false">(G64-E64)/6</f>
         <v>0</v>
       </c>
-      <c r="K64" s="13" t="n">
+      <c r="K64" s="11" t="n">
         <f aca="false">J64*J64</f>
         <v>0</v>
       </c>
       <c r="P64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B65" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" s="15" t="n">
+      <c r="A65" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C65" s="12"/>
+      <c r="D65" s="12"/>
+      <c r="E65" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G65" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H65" s="0"/>
@@ -2653,53 +2603,53 @@
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B66" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E66" s="13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E66" s="11" t="n">
         <f aca="false">E67</f>
         <v>0</v>
       </c>
-      <c r="F66" s="13" t="n">
+      <c r="F66" s="11" t="n">
         <f aca="false">F67</f>
         <v>0</v>
       </c>
-      <c r="G66" s="13" t="n">
+      <c r="G66" s="11" t="n">
         <f aca="false">G67</f>
         <v>0</v>
       </c>
-      <c r="I66" s="13" t="n">
+      <c r="I66" s="11" t="n">
         <f aca="false">(E66+4*F66+G66)/6</f>
         <v>0</v>
       </c>
-      <c r="J66" s="13" t="n">
+      <c r="J66" s="11" t="n">
         <f aca="false">(G66-E66)/6</f>
         <v>0</v>
       </c>
-      <c r="K66" s="13" t="n">
+      <c r="K66" s="11" t="n">
         <f aca="false">J66*J66</f>
         <v>0</v>
       </c>
       <c r="P66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B67" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" s="15" t="n">
+      <c r="A67" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B67" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F67" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G67" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H67" s="0"/>
@@ -2711,75 +2661,68 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B68" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C68" s="19"/>
-      <c r="D68" s="19"/>
-      <c r="E68" s="21" t="n">
+      <c r="A68" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B68" s="16"/>
+      <c r="C68" s="16"/>
+      <c r="D68" s="16"/>
+      <c r="E68" s="17" t="n">
         <f aca="false">E69</f>
         <v>0</v>
       </c>
-      <c r="F68" s="21" t="n">
+      <c r="F68" s="17" t="n">
         <f aca="false">F69</f>
         <v>0</v>
       </c>
-      <c r="G68" s="21" t="n">
+      <c r="G68" s="17" t="n">
         <f aca="false">G69</f>
         <v>0</v>
       </c>
-      <c r="H68" s="19"/>
-      <c r="I68" s="19"/>
-      <c r="J68" s="19"/>
-      <c r="K68" s="19"/>
+      <c r="H68" s="16"/>
+      <c r="I68" s="16"/>
+      <c r="J68" s="16"/>
+      <c r="K68" s="16"/>
       <c r="P68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B69" s="23" t="n">
-        <v>0</v>
-      </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="24" t="n">
+      <c r="A69" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="19" t="n">
         <f aca="false">E70</f>
         <v>0</v>
       </c>
-      <c r="F69" s="24" t="n">
+      <c r="F69" s="19" t="n">
         <f aca="false">F70</f>
         <v>0</v>
       </c>
-      <c r="G69" s="24" t="n">
+      <c r="G69" s="19" t="n">
         <f aca="false">G70</f>
         <v>0</v>
       </c>
-      <c r="H69" s="22"/>
-      <c r="I69" s="22"/>
-      <c r="J69" s="22"/>
-      <c r="K69" s="22"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+      <c r="J69" s="18"/>
+      <c r="K69" s="18"/>
       <c r="P69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E70" s="15" t="n">
+        <v>59</v>
+      </c>
+      <c r="E70" s="13" t="n">
         <f aca="false">E71</f>
         <v>0</v>
       </c>
-      <c r="F70" s="15" t="n">
+      <c r="F70" s="13" t="n">
         <f aca="false">F71</f>
         <v>0</v>
       </c>
-      <c r="G70" s="15" t="n">
+      <c r="G70" s="13" t="n">
         <f aca="false">G71</f>
         <v>0</v>
       </c>
@@ -2790,53 +2733,53 @@
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="13" t="n">
+        <v>60</v>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E71" s="11" t="n">
         <f aca="false">E72</f>
         <v>0</v>
       </c>
-      <c r="F71" s="13" t="n">
+      <c r="F71" s="11" t="n">
         <f aca="false">F72</f>
         <v>0</v>
       </c>
-      <c r="G71" s="13" t="n">
+      <c r="G71" s="11" t="n">
         <f aca="false">G72</f>
         <v>0</v>
       </c>
-      <c r="I71" s="13" t="n">
+      <c r="I71" s="11" t="n">
         <f aca="false">(E71+4*F71+G71)/6</f>
         <v>0</v>
       </c>
-      <c r="J71" s="13" t="n">
+      <c r="J71" s="11" t="n">
         <f aca="false">(G71-E71)/6</f>
         <v>0</v>
       </c>
-      <c r="K71" s="13" t="n">
+      <c r="K71" s="11" t="n">
         <f aca="false">J71*J71</f>
         <v>0</v>
       </c>
       <c r="P71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B72" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" s="15" t="n">
+      <c r="A72" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="B72" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C72" s="12"/>
+      <c r="D72" s="12"/>
+      <c r="E72" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G72" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H72" s="0"/>
@@ -2848,108 +2791,104 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="B73" s="17" t="n">
-        <v>0</v>
-      </c>
-      <c r="C73" s="16"/>
-      <c r="D73" s="16"/>
-      <c r="E73" s="18" t="n">
+      <c r="A73" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="15" t="n">
         <f aca="false">E74</f>
         <v>0</v>
       </c>
-      <c r="F73" s="18" t="n">
+      <c r="F73" s="15" t="n">
         <f aca="false">F74</f>
         <v>0</v>
       </c>
-      <c r="G73" s="18" t="n">
+      <c r="G73" s="15" t="n">
         <f aca="false">G74</f>
         <v>0</v>
       </c>
-      <c r="H73" s="16"/>
-      <c r="I73" s="16"/>
-      <c r="J73" s="16"/>
-      <c r="K73" s="16"/>
+      <c r="H73" s="14"/>
+      <c r="I73" s="14"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
       <c r="P73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="B74" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="C74" s="19"/>
-      <c r="D74" s="19"/>
-      <c r="E74" s="21" t="n">
+      <c r="A74" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="B74" s="16"/>
+      <c r="C74" s="16"/>
+      <c r="D74" s="16"/>
+      <c r="E74" s="17" t="n">
         <f aca="false">E75</f>
         <v>0</v>
       </c>
-      <c r="F74" s="21" t="n">
+      <c r="F74" s="17" t="n">
         <f aca="false">F75</f>
         <v>0</v>
       </c>
-      <c r="G74" s="21" t="n">
+      <c r="G74" s="17" t="n">
         <f aca="false">G75</f>
         <v>0</v>
       </c>
-      <c r="H74" s="19"/>
-      <c r="I74" s="19"/>
-      <c r="J74" s="19"/>
-      <c r="K74" s="19"/>
+      <c r="H74" s="16"/>
+      <c r="I74" s="16"/>
+      <c r="J74" s="16"/>
+      <c r="K74" s="16"/>
       <c r="P74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="13" t="n">
+        <v>58</v>
+      </c>
+      <c r="B75" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E75" s="11" t="n">
         <f aca="false">E76</f>
         <v>0</v>
       </c>
-      <c r="F75" s="13" t="n">
+      <c r="F75" s="11" t="n">
         <f aca="false">F76</f>
         <v>0</v>
       </c>
-      <c r="G75" s="13" t="n">
+      <c r="G75" s="11" t="n">
         <f aca="false">G76</f>
         <v>0</v>
       </c>
-      <c r="I75" s="13" t="n">
+      <c r="I75" s="11" t="n">
         <f aca="false">(E75+4*F75+G75)/6</f>
         <v>0</v>
       </c>
-      <c r="J75" s="13" t="n">
+      <c r="J75" s="11" t="n">
         <f aca="false">(G75-E75)/6</f>
         <v>0</v>
       </c>
-      <c r="K75" s="13" t="n">
+      <c r="K75" s="11" t="n">
         <f aca="false">J75*J75</f>
         <v>0</v>
       </c>
       <c r="P75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="B76" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" s="15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" s="15" t="n">
+      <c r="A76" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="B76" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
+      <c r="E76" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G76" s="13" t="n">
         <v>0</v>
       </c>
       <c r="H76" s="0"/>
@@ -2974,115 +2913,115 @@
       <c r="K77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" s="25"/>
-      <c r="C78" s="25"/>
-      <c r="D78" s="25"/>
-      <c r="E78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(E2:E76,B2:B76)</f>
+      <c r="A78" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B78" s="20"/>
+      <c r="C78" s="20"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(E2:E77,B2:B77)</f>
         <v>27</v>
       </c>
-      <c r="F78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(F2:F76,B2:B76)</f>
+      <c r="F78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(F2:F77,B2:B77)</f>
         <v>54</v>
       </c>
-      <c r="G78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(G2:G76,B2:B76)</f>
+      <c r="G78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(G2:G77,B2:B77)</f>
         <v>103</v>
       </c>
-      <c r="H78" s="25"/>
-      <c r="I78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(I2:I76,B2:B76)</f>
+      <c r="H78" s="20"/>
+      <c r="I78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(I2:I77,B2:B77)</f>
         <v>57.6666666666667</v>
       </c>
-      <c r="J78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(J2:J76,B2:B76)</f>
+      <c r="J78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(J2:J77,B2:B77)</f>
         <v>12.6666666666667</v>
       </c>
-      <c r="K78" s="26" t="n">
-        <f aca="false">SUMPRODUCT(K2:K76,B2:B76)</f>
+      <c r="K78" s="21" t="n">
+        <f aca="false">SUMPRODUCT(K2:K77,B2:B77)</f>
         <v>13.2777777777778</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="B79" s="25"/>
-      <c r="C79" s="25"/>
-      <c r="D79" s="25"/>
-      <c r="E79" s="26" t="n">
-        <f aca="false">SUMPRODUCT(E2:E76,M2:M76)</f>
-        <v>1</v>
-      </c>
-      <c r="F79" s="26" t="n">
-        <f aca="false">SUMPRODUCT(F2:F76,M2:M76)</f>
-        <v>1</v>
-      </c>
-      <c r="G79" s="26" t="n">
-        <f aca="false">SUMPRODUCT(G2:G76,M2:M76)</f>
+      <c r="A79" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="B79" s="20"/>
+      <c r="C79" s="20"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="21" t="n">
+        <f aca="false">SUMPRODUCT(E2:E77,M2:M77)</f>
+        <v>1</v>
+      </c>
+      <c r="F79" s="21" t="n">
+        <f aca="false">SUMPRODUCT(F2:F77,M2:M77)</f>
+        <v>1</v>
+      </c>
+      <c r="G79" s="21" t="n">
+        <f aca="false">SUMPRODUCT(G2:G77,M2:M77)</f>
         <v>2</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="B80" s="25"/>
-      <c r="C80" s="25"/>
-      <c r="D80" s="25"/>
-      <c r="E80" s="26" t="n">
-        <f aca="false">SUMPRODUCT(E2:E76,N2:N76)</f>
+      <c r="A80" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B80" s="20"/>
+      <c r="C80" s="20"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21" t="n">
+        <f aca="false">SUMPRODUCT(E2:E77,N2:N77)</f>
         <v>20</v>
       </c>
-      <c r="F80" s="26" t="n">
-        <f aca="false">SUMPRODUCT(F2:F76,N2:N76)</f>
+      <c r="F80" s="21" t="n">
+        <f aca="false">SUMPRODUCT(F2:F77,N2:N77)</f>
         <v>35</v>
       </c>
-      <c r="G80" s="26" t="n">
-        <f aca="false">SUMPRODUCT(G2:G76,N2:N76)</f>
+      <c r="G80" s="21" t="n">
+        <f aca="false">SUMPRODUCT(G2:G77,N2:N77)</f>
         <v>61</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="B81" s="25"/>
-      <c r="C81" s="25"/>
-      <c r="D81" s="25"/>
-      <c r="E81" s="26" t="n">
-        <f aca="false">SUMPRODUCT(E2:E76,O2:O76)</f>
+      <c r="A81" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81" s="20"/>
+      <c r="C81" s="20"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21" t="n">
+        <f aca="false">SUMPRODUCT(E2:E77,O2:O77)</f>
         <v>6</v>
       </c>
-      <c r="F81" s="26" t="n">
-        <f aca="false">SUMPRODUCT(F2:F76,O2:O76)</f>
+      <c r="F81" s="21" t="n">
+        <f aca="false">SUMPRODUCT(F2:F77,O2:O77)</f>
         <v>18</v>
       </c>
-      <c r="G81" s="26" t="n">
-        <f aca="false">SUMPRODUCT(G2:G76,O2:O76)</f>
+      <c r="G81" s="21" t="n">
+        <f aca="false">SUMPRODUCT(G2:G77,O2:O77)</f>
         <v>40</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
-      <c r="E82" s="26" t="n">
-        <f aca="false">SUMPRODUCT(E2:E76,P2:P76)</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="26" t="n">
-        <f aca="false">SUMPRODUCT(F2:F76,P2:P76)</f>
-        <v>0</v>
-      </c>
-      <c r="G82" s="26" t="n">
-        <f aca="false">SUMPRODUCT(G2:G76,P2:P76)</f>
+      <c r="A82" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B82" s="20"/>
+      <c r="C82" s="20"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="21" t="n">
+        <f aca="false">SUMPRODUCT(E2:E77,P2:P77)</f>
+        <v>0</v>
+      </c>
+      <c r="F82" s="21" t="n">
+        <f aca="false">SUMPRODUCT(F2:F77,P2:P77)</f>
+        <v>0</v>
+      </c>
+      <c r="G82" s="21" t="n">
+        <f aca="false">SUMPRODUCT(G2:G77,P2:P77)</f>
         <v>0</v>
       </c>
     </row>
@@ -3093,56 +3032,56 @@
       <c r="D83" s="0"/>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="27" t="s">
-        <v>70</v>
+      <c r="A84" s="22" t="s">
+        <v>71</v>
       </c>
       <c r="B84" s="0"/>
-      <c r="C84" s="13" t="n">
+      <c r="C84" s="11" t="n">
         <f aca="false">SQRT(K78)</f>
         <v>3.64386851817924</v>
       </c>
       <c r="D84" s="0"/>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="27" t="s">
-        <v>71</v>
+      <c r="A85" s="22" t="s">
+        <v>72</v>
       </c>
       <c r="B85" s="0"/>
-      <c r="C85" s="13" t="n">
+      <c r="C85" s="11" t="n">
         <v>1.5</v>
       </c>
       <c r="D85" s="0"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B86" s="25"/>
-      <c r="C86" s="26" t="n">
+      <c r="A86" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B86" s="20"/>
+      <c r="C86" s="21" t="n">
         <f aca="false">I78-2*C84</f>
         <v>50.3789296303082</v>
       </c>
-      <c r="D86" s="28" t="n">
+      <c r="D86" s="23" t="n">
         <f aca="false">C86*C85</f>
         <v>75.5683944454623</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="B87" s="25"/>
-      <c r="C87" s="26" t="n">
+      <c r="A87" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B87" s="20"/>
+      <c r="C87" s="21" t="n">
         <f aca="false">I78+2*C84</f>
         <v>64.9544037030251</v>
       </c>
-      <c r="D87" s="28" t="n">
+      <c r="D87" s="23" t="n">
         <f aca="false">C87*C85</f>
         <v>97.4316055545377</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K76"/>
+  <autoFilter ref="A1:K77"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
improvements: samples files have been updated
</commit_message>
<xml_diff>
--- a/example/Estimation Tool.mm.f.xlsx
+++ b/example/Estimation Tool.mm.f.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$77</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$K$56</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="59">
   <si>
     <t xml:space="preserve">Task / Subtask</t>
   </si>
@@ -62,9 +62,6 @@
     <t xml:space="preserve">(coding)</t>
   </si>
   <si>
-    <t xml:space="preserve">(test)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Stage 1: Implement the Idea</t>
   </si>
   <si>
@@ -185,45 +182,6 @@
     <t xml:space="preserve">  Analyze feedbacks</t>
   </si>
   <si>
-    <t xml:space="preserve">...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">this is a temporary branch for theme testing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                ...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                  (test)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">              (test)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          (test)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Total</t>
   </si>
   <si>
@@ -234,9 +192,6 @@
   </si>
   <si>
     <t xml:space="preserve">  - coding</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  - test</t>
   </si>
   <si>
     <t xml:space="preserve">Standard deviation</t>
@@ -310,7 +265,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,31 +281,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD6E1E9"/>
-        <bgColor rgb="FFE0E9EF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0E9EF"/>
-        <bgColor rgb="FFEBF0F4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEBF0F4"/>
-        <bgColor rgb="FFF4EFEB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF5F8FA"/>
-        <bgColor rgb="FFEBF0F4"/>
+        <bgColor rgb="FFE9DED6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF4EFEB"/>
-        <bgColor rgb="FFEBF0F4"/>
+        <bgColor rgb="FFE9DED6"/>
       </patternFill>
     </fill>
     <fill>
@@ -401,7 +338,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="18">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -458,35 +395,11 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -494,7 +407,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -510,7 +423,7 @@
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFF5F8FA"/>
+      <rgbColor rgb="FFF4EFEB"/>
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
@@ -527,8 +440,8 @@
       <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFF4EFEB"/>
-      <rgbColor rgb="FFE0E9EF"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -542,7 +455,7 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFEBF0F4"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
@@ -579,7 +492,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P87"/>
+  <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -595,8 +508,8 @@
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
     <col collapsed="false" hidden="false" max="11" min="9" style="3" width="7.56122448979592"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="true" max="16" min="13" style="1" width="0"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="true" max="15" min="13" style="1" width="0"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,18 +551,15 @@
       <c r="O1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="7" t="n">
         <f aca="false">E3+E12+E17+E19</f>
@@ -670,11 +580,10 @@
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -698,11 +607,10 @@
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
       <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>1</v>
@@ -734,11 +642,10 @@
       <c r="M4" s="0"/>
       <c r="N4" s="0"/>
       <c r="O4" s="0"/>
-      <c r="P4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="12" t="n">
         <v>0</v>
@@ -763,11 +670,10 @@
         <v>1</v>
       </c>
       <c r="O5" s="0"/>
-      <c r="P5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -799,11 +705,10 @@
       <c r="M6" s="0"/>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
-      <c r="P6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="12" t="n">
         <v>0</v>
@@ -828,11 +733,10 @@
         <v>1</v>
       </c>
       <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>1</v>
@@ -864,11 +768,10 @@
       <c r="M8" s="0"/>
       <c r="N8" s="0"/>
       <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="12" t="n">
         <v>0</v>
@@ -893,11 +796,10 @@
         <v>1</v>
       </c>
       <c r="O9" s="0"/>
-      <c r="P9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>1</v>
@@ -929,11 +831,10 @@
       <c r="M10" s="0"/>
       <c r="N10" s="0"/>
       <c r="O10" s="0"/>
-      <c r="P10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="12" t="n">
         <v>0</v>
@@ -958,11 +859,10 @@
         <v>1</v>
       </c>
       <c r="O11" s="0"/>
-      <c r="P11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="8"/>
@@ -986,11 +886,10 @@
       <c r="M12" s="0"/>
       <c r="N12" s="0"/>
       <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>1</v>
@@ -1022,11 +921,10 @@
       <c r="M13" s="0"/>
       <c r="N13" s="0"/>
       <c r="O13" s="0"/>
-      <c r="P13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="12" t="n">
         <v>0</v>
@@ -1051,11 +949,10 @@
       <c r="O14" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>1</v>
@@ -1087,11 +984,10 @@
       <c r="M15" s="0"/>
       <c r="N15" s="0"/>
       <c r="O15" s="0"/>
-      <c r="P15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="12" t="n">
         <v>0</v>
@@ -1116,11 +1012,10 @@
       <c r="O16" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>1</v>
@@ -1152,11 +1047,10 @@
       <c r="M17" s="0"/>
       <c r="N17" s="0"/>
       <c r="O17" s="0"/>
-      <c r="P17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="12" t="n">
         <v>0</v>
@@ -1181,11 +1075,10 @@
         <v>1</v>
       </c>
       <c r="O18" s="0"/>
-      <c r="P18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>1</v>
@@ -1217,11 +1110,10 @@
       <c r="M19" s="0"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
-      <c r="P19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20" s="12" t="n">
         <v>0</v>
@@ -1246,16 +1138,15 @@
         <v>1</v>
       </c>
       <c r="O20" s="0"/>
-      <c r="P20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
       <c r="D21" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E21" s="7" t="n">
         <f aca="false">E22+E29+E32</f>
@@ -1276,16 +1167,15 @@
       <c r="M21" s="0"/>
       <c r="N21" s="0"/>
       <c r="O21" s="0"/>
-      <c r="P21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
       <c r="D22" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="10" t="n">
         <f aca="false">E23+E25+E27</f>
@@ -1306,11 +1196,10 @@
       <c r="M22" s="0"/>
       <c r="N22" s="0"/>
       <c r="O22" s="0"/>
-      <c r="P22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>1</v>
@@ -1342,11 +1231,10 @@
       <c r="M23" s="0"/>
       <c r="N23" s="0"/>
       <c r="O23" s="0"/>
-      <c r="P23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B24" s="12" t="n">
         <v>0</v>
@@ -1371,11 +1259,10 @@
         <v>1</v>
       </c>
       <c r="O24" s="0"/>
-      <c r="P24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>1</v>
@@ -1407,11 +1294,10 @@
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
       <c r="O25" s="0"/>
-      <c r="P25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B26" s="12" t="n">
         <v>0</v>
@@ -1436,11 +1322,10 @@
         <v>1</v>
       </c>
       <c r="O26" s="0"/>
-      <c r="P26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>1</v>
@@ -1472,11 +1357,10 @@
       <c r="M27" s="0"/>
       <c r="N27" s="0"/>
       <c r="O27" s="0"/>
-      <c r="P27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="12" t="n">
         <v>0</v>
@@ -1501,11 +1385,10 @@
         <v>1</v>
       </c>
       <c r="O28" s="0"/>
-      <c r="P28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>1</v>
@@ -1537,11 +1420,10 @@
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
       <c r="O29" s="0"/>
-      <c r="P29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B30" s="12" t="n">
         <v>0</v>
@@ -1566,11 +1448,10 @@
         <v>1</v>
       </c>
       <c r="O30" s="0"/>
-      <c r="P30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" s="12" t="n">
         <v>0</v>
@@ -1595,11 +1476,10 @@
       <c r="O31" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>1</v>
@@ -1631,11 +1511,10 @@
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
       <c r="O32" s="0"/>
-      <c r="P32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B33" s="12" t="n">
         <v>0</v>
@@ -1660,11 +1539,10 @@
         <v>1</v>
       </c>
       <c r="O33" s="0"/>
-      <c r="P33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B34" s="12" t="n">
         <v>0</v>
@@ -1689,16 +1567,15 @@
       <c r="O34" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E35" s="7" t="n">
         <f aca="false">E36+E41+E43+E45+E47</f>
@@ -1719,11 +1596,10 @@
       <c r="M35" s="0"/>
       <c r="N35" s="0"/>
       <c r="O35" s="0"/>
-      <c r="P35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -1747,11 +1623,10 @@
       <c r="M36" s="0"/>
       <c r="N36" s="0"/>
       <c r="O36" s="0"/>
-      <c r="P36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>1</v>
@@ -1783,11 +1658,10 @@
       <c r="M37" s="0"/>
       <c r="N37" s="0"/>
       <c r="O37" s="0"/>
-      <c r="P37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B38" s="12" t="n">
         <v>0</v>
@@ -1812,11 +1686,10 @@
       <c r="O38" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>1</v>
@@ -1848,11 +1721,10 @@
       <c r="M39" s="0"/>
       <c r="N39" s="0"/>
       <c r="O39" s="0"/>
-      <c r="P39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B40" s="12" t="n">
         <v>0</v>
@@ -1877,11 +1749,10 @@
       <c r="O40" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>1</v>
@@ -1913,11 +1784,10 @@
       <c r="M41" s="0"/>
       <c r="N41" s="0"/>
       <c r="O41" s="0"/>
-      <c r="P41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B42" s="12" t="n">
         <v>0</v>
@@ -1942,11 +1812,10 @@
       </c>
       <c r="N42" s="0"/>
       <c r="O42" s="0"/>
-      <c r="P42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>1</v>
@@ -1977,11 +1846,10 @@
       </c>
       <c r="N43" s="0"/>
       <c r="O43" s="0"/>
-      <c r="P43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B44" s="12" t="n">
         <v>0</v>
@@ -2005,11 +1873,10 @@
         <v>1</v>
       </c>
       <c r="O44" s="0"/>
-      <c r="P44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>1</v>
@@ -2040,11 +1907,10 @@
       </c>
       <c r="N45" s="0"/>
       <c r="O45" s="0"/>
-      <c r="P45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="12" t="n">
         <v>0</v>
@@ -2068,17 +1934,16 @@
         <v>1</v>
       </c>
       <c r="O46" s="0"/>
-      <c r="P46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B47" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>48</v>
       </c>
       <c r="E47" s="11" t="n">
         <f aca="false">E48</f>
@@ -2106,11 +1971,10 @@
       </c>
       <c r="N47" s="0"/>
       <c r="O47" s="0"/>
-      <c r="P47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" s="12" t="n">
         <v>0</v>
@@ -2134,16 +1998,15 @@
         <v>1</v>
       </c>
       <c r="O48" s="0"/>
-      <c r="P48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E49" s="7" t="n">
         <f aca="false">E50+E52+E54</f>
@@ -2163,11 +2026,10 @@
       <c r="K49" s="5"/>
       <c r="N49" s="0"/>
       <c r="O49" s="0"/>
-      <c r="P49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>1</v>
@@ -2198,11 +2060,10 @@
       </c>
       <c r="N50" s="0"/>
       <c r="O50" s="0"/>
-      <c r="P50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B51" s="12" t="n">
         <v>0</v>
@@ -2226,11 +2087,10 @@
         <v>1</v>
       </c>
       <c r="O51" s="0"/>
-      <c r="P51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>1</v>
@@ -2261,11 +2121,10 @@
       </c>
       <c r="N52" s="0"/>
       <c r="O52" s="0"/>
-      <c r="P52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B53" s="12" t="n">
         <v>0</v>
@@ -2289,11 +2148,10 @@
         <v>1</v>
       </c>
       <c r="O53" s="0"/>
-      <c r="P53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>1</v>
@@ -2323,11 +2181,10 @@
         <v>6.25</v>
       </c>
       <c r="O54" s="0"/>
-      <c r="P54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B55" s="12" t="n">
         <v>0</v>
@@ -2350,738 +2207,170 @@
       <c r="O55" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="P55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B56" s="5"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="6" t="s">
+      <c r="A56" s="0"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="0"/>
+      <c r="E56" s="0"/>
+      <c r="F56" s="0"/>
+      <c r="G56" s="0"/>
+      <c r="H56" s="0"/>
+      <c r="I56" s="0"/>
+      <c r="J56" s="0"/>
+      <c r="K56" s="0"/>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(E2:E56,B2:B56)</f>
+        <v>27</v>
+      </c>
+      <c r="F57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(F2:F56,B2:B56)</f>
         <v>54</v>
       </c>
-      <c r="E56" s="7" t="n">
-        <f aca="false">E57</f>
-        <v>0</v>
-      </c>
-      <c r="F56" s="7" t="n">
-        <f aca="false">F57</f>
-        <v>0</v>
-      </c>
-      <c r="G56" s="7" t="n">
-        <f aca="false">G57</f>
-        <v>0</v>
-      </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="5"/>
-      <c r="K56" s="5"/>
-      <c r="P56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" s="8"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="10" t="n">
-        <f aca="false">E58+E73</f>
-        <v>0</v>
-      </c>
-      <c r="F57" s="10" t="n">
-        <f aca="false">F58+F73</f>
-        <v>0</v>
-      </c>
-      <c r="G57" s="10" t="n">
-        <f aca="false">G58+G73</f>
-        <v>0</v>
-      </c>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="P57" s="0"/>
+      <c r="G57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(G2:G56,B2:B56)</f>
+        <v>103</v>
+      </c>
+      <c r="H57" s="14"/>
+      <c r="I57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(I2:I56,B2:B56)</f>
+        <v>57.6666666666667</v>
+      </c>
+      <c r="J57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(J2:J56,B2:B56)</f>
+        <v>12.6666666666667</v>
+      </c>
+      <c r="K57" s="15" t="n">
+        <f aca="false">SUMPRODUCT(K2:K56,B2:B56)</f>
+        <v>13.2777777777778</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="14" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B58" s="14"/>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
       <c r="E58" s="15" t="n">
-        <f aca="false">E59+E68</f>
-        <v>0</v>
+        <f aca="false">SUMPRODUCT(E2:E56,M2:M56)</f>
+        <v>1</v>
       </c>
       <c r="F58" s="15" t="n">
-        <f aca="false">F59+F68</f>
-        <v>0</v>
+        <f aca="false">SUMPRODUCT(F2:F56,M2:M56)</f>
+        <v>1</v>
       </c>
       <c r="G58" s="15" t="n">
-        <f aca="false">G59+G68</f>
-        <v>0</v>
-      </c>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-      <c r="K58" s="14"/>
-      <c r="P58" s="0"/>
+        <f aca="false">SUMPRODUCT(G2:G56,M2:M56)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15" t="n">
+        <f aca="false">SUMPRODUCT(E2:E56,N2:N56)</f>
+        <v>20</v>
+      </c>
+      <c r="F59" s="15" t="n">
+        <f aca="false">SUMPRODUCT(F2:F56,N2:N56)</f>
+        <v>35</v>
+      </c>
+      <c r="G59" s="15" t="n">
+        <f aca="false">SUMPRODUCT(G2:G56,N2:N56)</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="15" t="n">
+        <f aca="false">SUMPRODUCT(E2:E56,O2:O56)</f>
+        <v>6</v>
+      </c>
+      <c r="F60" s="15" t="n">
+        <f aca="false">SUMPRODUCT(F2:F56,O2:O56)</f>
+        <v>18</v>
+      </c>
+      <c r="G60" s="15" t="n">
+        <f aca="false">SUMPRODUCT(G2:G56,O2:O56)</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0"/>
+      <c r="B61" s="0"/>
+      <c r="C61" s="0"/>
+      <c r="D61" s="0"/>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B62" s="0"/>
+      <c r="C62" s="11" t="n">
+        <f aca="false">SQRT(K57)</f>
+        <v>3.64386851817924</v>
+      </c>
+      <c r="D62" s="0"/>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="16"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
-      <c r="E59" s="17" t="n">
-        <f aca="false">E60</f>
-        <v>0</v>
-      </c>
-      <c r="F59" s="17" t="n">
-        <f aca="false">F60</f>
-        <v>0</v>
-      </c>
-      <c r="G59" s="17" t="n">
-        <f aca="false">G60</f>
-        <v>0</v>
-      </c>
-      <c r="H59" s="16"/>
-      <c r="I59" s="16"/>
-      <c r="J59" s="16"/>
-      <c r="K59" s="16"/>
-      <c r="P59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="18" t="s">
+      <c r="B63" s="0"/>
+      <c r="C63" s="11" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="D63" s="0"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="18"/>
-      <c r="C60" s="18"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="19" t="n">
-        <f aca="false">E61</f>
-        <v>0</v>
-      </c>
-      <c r="F60" s="19" t="n">
-        <f aca="false">F61</f>
-        <v>0</v>
-      </c>
-      <c r="G60" s="19" t="n">
-        <f aca="false">G61</f>
-        <v>0</v>
-      </c>
-      <c r="H60" s="18"/>
-      <c r="I60" s="18"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="18"/>
-      <c r="P60" s="0"/>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E61" s="13" t="n">
-        <f aca="false">E62+E66</f>
-        <v>0</v>
-      </c>
-      <c r="F61" s="13" t="n">
-        <f aca="false">F62+F66</f>
-        <v>0</v>
-      </c>
-      <c r="G61" s="13" t="n">
-        <f aca="false">G62+G66</f>
-        <v>0</v>
-      </c>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="P61" s="0"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E62" s="13" t="n">
-        <f aca="false">E63</f>
-        <v>0</v>
-      </c>
-      <c r="F62" s="13" t="n">
-        <f aca="false">F63</f>
-        <v>0</v>
-      </c>
-      <c r="G62" s="13" t="n">
-        <f aca="false">G63</f>
-        <v>0</v>
-      </c>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="P62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E63" s="13" t="n">
-        <f aca="false">E64</f>
-        <v>0</v>
-      </c>
-      <c r="F63" s="13" t="n">
-        <f aca="false">F64</f>
-        <v>0</v>
-      </c>
-      <c r="G63" s="13" t="n">
-        <f aca="false">G64</f>
-        <v>0</v>
-      </c>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="P63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B64" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E64" s="11" t="n">
-        <f aca="false">E65</f>
-        <v>0</v>
-      </c>
-      <c r="F64" s="11" t="n">
-        <f aca="false">F65</f>
-        <v>0</v>
-      </c>
-      <c r="G64" s="11" t="n">
-        <f aca="false">G65</f>
-        <v>0</v>
-      </c>
-      <c r="I64" s="11" t="n">
-        <f aca="false">(E64+4*F64+G64)/6</f>
-        <v>0</v>
-      </c>
-      <c r="J64" s="11" t="n">
-        <f aca="false">(G64-E64)/6</f>
-        <v>0</v>
-      </c>
-      <c r="K64" s="11" t="n">
-        <f aca="false">J64*J64</f>
-        <v>0</v>
-      </c>
-      <c r="P64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B65" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C65" s="12"/>
-      <c r="D65" s="12"/>
-      <c r="E65" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G65" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H65" s="0"/>
-      <c r="I65" s="0"/>
-      <c r="J65" s="0"/>
-      <c r="K65" s="0"/>
-      <c r="P65" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B66" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E66" s="11" t="n">
-        <f aca="false">E67</f>
-        <v>0</v>
-      </c>
-      <c r="F66" s="11" t="n">
-        <f aca="false">F67</f>
-        <v>0</v>
-      </c>
-      <c r="G66" s="11" t="n">
-        <f aca="false">G67</f>
-        <v>0</v>
-      </c>
-      <c r="I66" s="11" t="n">
-        <f aca="false">(E66+4*F66+G66)/6</f>
-        <v>0</v>
-      </c>
-      <c r="J66" s="11" t="n">
-        <f aca="false">(G66-E66)/6</f>
-        <v>0</v>
-      </c>
-      <c r="K66" s="11" t="n">
-        <f aca="false">J66*J66</f>
-        <v>0</v>
-      </c>
-      <c r="P66" s="0"/>
-    </row>
-    <row r="67" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B67" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F67" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G67" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H67" s="0"/>
-      <c r="I67" s="0"/>
-      <c r="J67" s="0"/>
-      <c r="K67" s="0"/>
-      <c r="P67" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B68" s="16"/>
-      <c r="C68" s="16"/>
-      <c r="D68" s="16"/>
-      <c r="E68" s="17" t="n">
-        <f aca="false">E69</f>
-        <v>0</v>
-      </c>
-      <c r="F68" s="17" t="n">
-        <f aca="false">F69</f>
-        <v>0</v>
-      </c>
-      <c r="G68" s="17" t="n">
-        <f aca="false">G69</f>
-        <v>0</v>
-      </c>
-      <c r="H68" s="16"/>
-      <c r="I68" s="16"/>
-      <c r="J68" s="16"/>
-      <c r="K68" s="16"/>
-      <c r="P68" s="0"/>
-    </row>
-    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="18" t="s">
+      <c r="B64" s="14"/>
+      <c r="C64" s="15" t="n">
+        <f aca="false">I57-2*C62</f>
+        <v>50.3789296303082</v>
+      </c>
+      <c r="D64" s="17" t="n">
+        <f aca="false">C64*C63</f>
+        <v>75.5683944454623</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="19" t="n">
-        <f aca="false">E70</f>
-        <v>0</v>
-      </c>
-      <c r="F69" s="19" t="n">
-        <f aca="false">F70</f>
-        <v>0</v>
-      </c>
-      <c r="G69" s="19" t="n">
-        <f aca="false">G70</f>
-        <v>0</v>
-      </c>
-      <c r="H69" s="18"/>
-      <c r="I69" s="18"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="18"/>
-      <c r="P69" s="0"/>
-    </row>
-    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="E70" s="13" t="n">
-        <f aca="false">E71</f>
-        <v>0</v>
-      </c>
-      <c r="F70" s="13" t="n">
-        <f aca="false">F71</f>
-        <v>0</v>
-      </c>
-      <c r="G70" s="13" t="n">
-        <f aca="false">G71</f>
-        <v>0</v>
-      </c>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="P70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B71" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E71" s="11" t="n">
-        <f aca="false">E72</f>
-        <v>0</v>
-      </c>
-      <c r="F71" s="11" t="n">
-        <f aca="false">F72</f>
-        <v>0</v>
-      </c>
-      <c r="G71" s="11" t="n">
-        <f aca="false">G72</f>
-        <v>0</v>
-      </c>
-      <c r="I71" s="11" t="n">
-        <f aca="false">(E71+4*F71+G71)/6</f>
-        <v>0</v>
-      </c>
-      <c r="J71" s="11" t="n">
-        <f aca="false">(G71-E71)/6</f>
-        <v>0</v>
-      </c>
-      <c r="K71" s="11" t="n">
-        <f aca="false">J71*J71</f>
-        <v>0</v>
-      </c>
-      <c r="P71" s="0"/>
-    </row>
-    <row r="72" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="B72" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12"/>
-      <c r="E72" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G72" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H72" s="0"/>
-      <c r="I72" s="0"/>
-      <c r="J72" s="0"/>
-      <c r="K72" s="0"/>
-      <c r="P72" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B73" s="14"/>
-      <c r="C73" s="14"/>
-      <c r="D73" s="14"/>
-      <c r="E73" s="15" t="n">
-        <f aca="false">E74</f>
-        <v>0</v>
-      </c>
-      <c r="F73" s="15" t="n">
-        <f aca="false">F74</f>
-        <v>0</v>
-      </c>
-      <c r="G73" s="15" t="n">
-        <f aca="false">G74</f>
-        <v>0</v>
-      </c>
-      <c r="H73" s="14"/>
-      <c r="I73" s="14"/>
-      <c r="J73" s="14"/>
-      <c r="K73" s="14"/>
-      <c r="P73" s="0"/>
-    </row>
-    <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B74" s="16"/>
-      <c r="C74" s="16"/>
-      <c r="D74" s="16"/>
-      <c r="E74" s="17" t="n">
-        <f aca="false">E75</f>
-        <v>0</v>
-      </c>
-      <c r="F74" s="17" t="n">
-        <f aca="false">F75</f>
-        <v>0</v>
-      </c>
-      <c r="G74" s="17" t="n">
-        <f aca="false">G75</f>
-        <v>0</v>
-      </c>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-      <c r="J74" s="16"/>
-      <c r="K74" s="16"/>
-      <c r="P74" s="0"/>
-    </row>
-    <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B75" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E75" s="11" t="n">
-        <f aca="false">E76</f>
-        <v>0</v>
-      </c>
-      <c r="F75" s="11" t="n">
-        <f aca="false">F76</f>
-        <v>0</v>
-      </c>
-      <c r="G75" s="11" t="n">
-        <f aca="false">G76</f>
-        <v>0</v>
-      </c>
-      <c r="I75" s="11" t="n">
-        <f aca="false">(E75+4*F75+G75)/6</f>
-        <v>0</v>
-      </c>
-      <c r="J75" s="11" t="n">
-        <f aca="false">(G75-E75)/6</f>
-        <v>0</v>
-      </c>
-      <c r="K75" s="11" t="n">
-        <f aca="false">J75*J75</f>
-        <v>0</v>
-      </c>
-      <c r="P75" s="0"/>
-    </row>
-    <row r="76" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B76" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12"/>
-      <c r="E76" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G76" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" s="0"/>
-      <c r="I76" s="0"/>
-      <c r="J76" s="0"/>
-      <c r="K76" s="0"/>
-      <c r="P76" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0"/>
-      <c r="B77" s="0"/>
-      <c r="C77" s="0"/>
-      <c r="D77" s="0"/>
-      <c r="E77" s="0"/>
-      <c r="F77" s="0"/>
-      <c r="G77" s="0"/>
-      <c r="H77" s="0"/>
-      <c r="I77" s="0"/>
-      <c r="J77" s="0"/>
-      <c r="K77" s="0"/>
-    </row>
-    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B78" s="20"/>
-      <c r="C78" s="20"/>
-      <c r="D78" s="20"/>
-      <c r="E78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(E2:E77,B2:B77)</f>
-        <v>27</v>
-      </c>
-      <c r="F78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(F2:F77,B2:B77)</f>
-        <v>54</v>
-      </c>
-      <c r="G78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(G2:G77,B2:B77)</f>
-        <v>103</v>
-      </c>
-      <c r="H78" s="20"/>
-      <c r="I78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(I2:I77,B2:B77)</f>
-        <v>57.6666666666667</v>
-      </c>
-      <c r="J78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(J2:J77,B2:B77)</f>
-        <v>12.6666666666667</v>
-      </c>
-      <c r="K78" s="21" t="n">
-        <f aca="false">SUMPRODUCT(K2:K77,B2:B77)</f>
-        <v>13.2777777777778</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B79" s="20"/>
-      <c r="C79" s="20"/>
-      <c r="D79" s="20"/>
-      <c r="E79" s="21" t="n">
-        <f aca="false">SUMPRODUCT(E2:E77,M2:M77)</f>
-        <v>1</v>
-      </c>
-      <c r="F79" s="21" t="n">
-        <f aca="false">SUMPRODUCT(F2:F77,M2:M77)</f>
-        <v>1</v>
-      </c>
-      <c r="G79" s="21" t="n">
-        <f aca="false">SUMPRODUCT(G2:G77,M2:M77)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="B80" s="20"/>
-      <c r="C80" s="20"/>
-      <c r="D80" s="20"/>
-      <c r="E80" s="21" t="n">
-        <f aca="false">SUMPRODUCT(E2:E77,N2:N77)</f>
-        <v>20</v>
-      </c>
-      <c r="F80" s="21" t="n">
-        <f aca="false">SUMPRODUCT(F2:F77,N2:N77)</f>
-        <v>35</v>
-      </c>
-      <c r="G80" s="21" t="n">
-        <f aca="false">SUMPRODUCT(G2:G77,N2:N77)</f>
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="B81" s="20"/>
-      <c r="C81" s="20"/>
-      <c r="D81" s="20"/>
-      <c r="E81" s="21" t="n">
-        <f aca="false">SUMPRODUCT(E2:E77,O2:O77)</f>
-        <v>6</v>
-      </c>
-      <c r="F81" s="21" t="n">
-        <f aca="false">SUMPRODUCT(F2:F77,O2:O77)</f>
-        <v>18</v>
-      </c>
-      <c r="G81" s="21" t="n">
-        <f aca="false">SUMPRODUCT(G2:G77,O2:O77)</f>
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B82" s="20"/>
-      <c r="C82" s="20"/>
-      <c r="D82" s="20"/>
-      <c r="E82" s="21" t="n">
-        <f aca="false">SUMPRODUCT(E2:E77,P2:P77)</f>
-        <v>0</v>
-      </c>
-      <c r="F82" s="21" t="n">
-        <f aca="false">SUMPRODUCT(F2:F77,P2:P77)</f>
-        <v>0</v>
-      </c>
-      <c r="G82" s="21" t="n">
-        <f aca="false">SUMPRODUCT(G2:G77,P2:P77)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0"/>
-      <c r="B83" s="0"/>
-      <c r="C83" s="0"/>
-      <c r="D83" s="0"/>
-    </row>
-    <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="B84" s="0"/>
-      <c r="C84" s="11" t="n">
-        <f aca="false">SQRT(K78)</f>
-        <v>3.64386851817924</v>
-      </c>
-      <c r="D84" s="0"/>
-    </row>
-    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="B85" s="0"/>
-      <c r="C85" s="11" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="D85" s="0"/>
-    </row>
-    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B86" s="20"/>
-      <c r="C86" s="21" t="n">
-        <f aca="false">I78-2*C84</f>
-        <v>50.3789296303082</v>
-      </c>
-      <c r="D86" s="23" t="n">
-        <f aca="false">C86*C85</f>
-        <v>75.5683944454623</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B87" s="20"/>
-      <c r="C87" s="21" t="n">
-        <f aca="false">I78+2*C84</f>
+      <c r="B65" s="14"/>
+      <c r="C65" s="15" t="n">
+        <f aca="false">I57+2*C62</f>
         <v>64.9544037030251</v>
       </c>
-      <c r="D87" s="23" t="n">
-        <f aca="false">C87*C85</f>
+      <c r="D65" s="17" t="n">
+        <f aca="false">C65*C63</f>
         <v>97.4316055545377</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K77"/>
+  <autoFilter ref="A1:K56"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>